<commit_message>
xl week 3 files
</commit_message>
<xml_diff>
--- a/static/output/Excel/LRcountsxl1-sol1.xlsx
+++ b/static/output/Excel/LRcountsxl1-sol1.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adolphus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bavanzi/Dropbox/Mac (3)/Documents/GitHub/ACTL20004-ACTL90021-Tutorials/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F82C26C-04E6-47E4-8201-B5F6C3CD8E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F365533E-1AAC-484F-AC2E-1546AD7E23F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
     <sheet name="Exposure" sheetId="3" r:id="rId2"/>
     <sheet name="IBNR" sheetId="4" r:id="rId3"/>
-    <sheet name="comparison" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>sum from 16</t>
   </si>
@@ -166,21 +165,6 @@
   </si>
   <si>
     <t>Period of</t>
-  </si>
-  <si>
-    <t>True rectangle:</t>
-  </si>
-  <si>
-    <t>A/E</t>
-  </si>
-  <si>
-    <t>Ultimate</t>
-  </si>
-  <si>
-    <t>Heatmap of A/E:</t>
-  </si>
-  <si>
-    <t>(average)</t>
   </si>
 </sst>
 </file>
@@ -346,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -383,11 +367,10 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -405,7 +388,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1087,7 +1070,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1811,7 +1794,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4485,9 +4468,9 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>2148</v>
       </c>
@@ -4540,7 +4523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2064</v>
       </c>
@@ -4593,7 +4576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1996</v>
       </c>
@@ -4646,7 +4629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2131</v>
       </c>
@@ -4699,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2033</v>
       </c>
@@ -4752,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2144</v>
       </c>
@@ -4805,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2073</v>
       </c>
@@ -4858,7 +4841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1958</v>
       </c>
@@ -4911,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2137</v>
       </c>
@@ -4964,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1858</v>
       </c>
@@ -5017,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2076</v>
       </c>
@@ -5070,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2027</v>
       </c>
@@ -5123,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -5176,7 +5159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -5229,7 +5212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1809</v>
       </c>
@@ -5282,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1879</v>
       </c>
@@ -5348,13 +5331,13 @@
       <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="18" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="18" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>24</v>
       </c>
@@ -5376,7 +5359,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>21</v>
       </c>
@@ -5435,7 +5418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="14"/>
       <c r="C3" s="1"/>
@@ -5451,7 +5434,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>0</v>
       </c>
@@ -5524,7 +5507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -5594,7 +5577,7 @@
       </c>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>2</v>
       </c>
@@ -5661,7 +5644,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>3</v>
       </c>
@@ -5725,7 +5708,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>4</v>
       </c>
@@ -5786,7 +5769,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>5</v>
       </c>
@@ -5844,7 +5827,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>6</v>
       </c>
@@ -5899,7 +5882,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>7</v>
       </c>
@@ -5951,7 +5934,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>8</v>
       </c>
@@ -6000,7 +5983,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>9</v>
       </c>
@@ -6046,7 +6029,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>10</v>
       </c>
@@ -6089,7 +6072,7 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <v>11</v>
       </c>
@@ -6129,7 +6112,7 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>12</v>
       </c>
@@ -6166,7 +6149,7 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>13</v>
       </c>
@@ -6200,7 +6183,7 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>14</v>
       </c>
@@ -6231,7 +6214,7 @@
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>15</v>
       </c>
@@ -6259,7 +6242,7 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
     </row>
-    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -6274,7 +6257,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -6294,7 +6277,7 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -6311,7 +6294,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -6326,7 +6309,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -6396,7 +6379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -6411,7 +6394,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -6466,7 +6449,7 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -6481,7 +6464,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -6543,7 +6526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -6559,7 +6542,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -6575,7 +6558,7 @@
       <c r="M30" s="5"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -6645,7 +6628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -6663,7 +6646,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -6679,7 +6662,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>13</v>
       </c>
@@ -6740,7 +6723,7 @@
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
     </row>
-    <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
@@ -6758,7 +6741,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -6774,7 +6757,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -6790,7 +6773,7 @@
       <c r="M37" s="5"/>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>11</v>
       </c>
@@ -6808,7 +6791,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -6825,7 +6808,7 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
@@ -6855,7 +6838,7 @@
       </c>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -6873,7 +6856,7 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -6911,7 +6894,7 @@
         <v>-2.7622278611067426</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -6949,7 +6932,7 @@
         <v>6.3150920044034262E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -6965,7 +6948,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>
@@ -6983,7 +6966,7 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
@@ -7004,7 +6987,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
@@ -7025,7 +7008,7 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -7046,7 +7029,7 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -7072,17 +7055,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFC4402-A461-4845-8A71-2163FA7D628A}">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="14" width="6.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="6.5" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>34</v>
       </c>
@@ -7109,7 +7092,7 @@
       </c>
       <c r="S1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>31</v>
       </c>
@@ -7171,7 +7154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="15"/>
       <c r="C3" s="1"/>
@@ -7192,7 +7175,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <f>Exposure!A4</f>
         <v>0</v>
@@ -7274,7 +7257,7 @@
         <v>9.2687091725423415E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <f>Exposure!A5</f>
         <v>1</v>
@@ -7356,7 +7339,7 @@
         <v>0.10178695747398346</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <f>Exposure!A6</f>
         <v>2</v>
@@ -7438,7 +7421,7 @@
         <v>9.1225136156930745E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <f>Exposure!A7</f>
         <v>3</v>
@@ -7520,7 +7503,7 @@
         <v>0.11031963674891716</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <f>Exposure!A8</f>
         <v>4</v>
@@ -7602,7 +7585,7 @@
         <v>0.10137085799904094</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <f>Exposure!A9</f>
         <v>5</v>
@@ -7684,7 +7667,7 @@
         <v>9.1523832795277052E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <f>Exposure!A10</f>
         <v>6</v>
@@ -7766,7 +7749,7 @@
         <v>9.5293669511178208E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <f>Exposure!A11</f>
         <v>7</v>
@@ -7848,7 +7831,7 @@
         <v>9.7176682326977556E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <f>Exposure!A12</f>
         <v>8</v>
@@ -7930,7 +7913,7 @@
         <v>8.4435144341872617E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <f>Exposure!A13</f>
         <v>9</v>
@@ -8012,7 +7995,7 @@
         <v>0.10498721201735624</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <f>Exposure!A14</f>
         <v>10</v>
@@ -8094,7 +8077,7 @@
         <v>9.5220154450587555E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <f>Exposure!A15</f>
         <v>11</v>
@@ -8176,7 +8159,7 @@
         <v>9.4716487164467442E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <f>Exposure!A16</f>
         <v>12</v>
@@ -8258,7 +8241,7 @@
         <v>9.8398261601542525E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <f>Exposure!A17</f>
         <v>13</v>
@@ -8340,7 +8323,7 @@
         <v>9.1356847238587904E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <f>Exposure!A18</f>
         <v>14</v>
@@ -8422,7 +8405,7 @@
         <v>9.5492518951464725E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <f>Exposure!A19</f>
         <v>15</v>
@@ -8504,7 +8487,7 @@
         <v>9.75599886655662E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -8525,7 +8508,7 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
     </row>
-    <row r="21" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -8549,15 +8532,15 @@
       </c>
       <c r="S21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="21"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -8577,7 +8560,7 @@
       <c r="S25" s="20"/>
       <c r="T25" s="19"/>
     </row>
-    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
@@ -8597,7 +8580,7 @@
       <c r="S26" s="20"/>
       <c r="T26" s="19"/>
     </row>
-    <row r="27" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -8617,7 +8600,7 @@
       <c r="S27" s="20"/>
       <c r="T27" s="19"/>
     </row>
-    <row r="28" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -8637,7 +8620,7 @@
       <c r="S28" s="20"/>
       <c r="T28" s="19"/>
     </row>
-    <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -8657,7 +8640,7 @@
       <c r="S29" s="20"/>
       <c r="T29" s="19"/>
     </row>
-    <row r="30" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -8677,7 +8660,7 @@
       <c r="S30" s="20"/>
       <c r="T30" s="19"/>
     </row>
-    <row r="31" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -8697,7 +8680,7 @@
       <c r="S31" s="20"/>
       <c r="T31" s="19"/>
     </row>
-    <row r="32" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -8717,7 +8700,7 @@
       <c r="S32" s="20"/>
       <c r="T32" s="19"/>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -8737,7 +8720,7 @@
       <c r="S33" s="20"/>
       <c r="T33" s="19"/>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
@@ -8757,7 +8740,7 @@
       <c r="S34" s="20"/>
       <c r="T34" s="19"/>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -8777,7 +8760,7 @@
       <c r="S35" s="20"/>
       <c r="T35" s="19"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -8797,7 +8780,7 @@
       <c r="S36" s="20"/>
       <c r="T36" s="19"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -8817,7 +8800,7 @@
       <c r="S37" s="20"/>
       <c r="T37" s="19"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
@@ -8837,7 +8820,7 @@
       <c r="S38" s="20"/>
       <c r="T38" s="19"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -8857,7 +8840,7 @@
       <c r="S39" s="20"/>
       <c r="T39" s="19"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -8877,13 +8860,13 @@
       <c r="S40" s="20"/>
       <c r="T40" s="19"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="P41" s="1"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="19"/>
       <c r="S41" s="3"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="21"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="20"/>
@@ -8892,7 +8875,7 @@
       <c r="T42" s="18"/>
       <c r="U42" s="18"/>
     </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C60" t="str">
         <f t="shared" ref="C60:O60" si="4">IF(C42&gt;0,C21/C42,"")</f>
         <v/>
@@ -8962,1456 +8945,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A43E3F-8704-49B9-A6D7-F74833BAC4DB}">
-  <dimension ref="A1:U35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="22">
-        <v>4</v>
-      </c>
-      <c r="D2" s="22">
-        <v>46</v>
-      </c>
-      <c r="E2" s="22">
-        <v>44</v>
-      </c>
-      <c r="F2" s="22">
-        <v>40</v>
-      </c>
-      <c r="G2" s="22">
-        <v>35</v>
-      </c>
-      <c r="H2" s="22">
-        <v>17</v>
-      </c>
-      <c r="I2" s="22">
-        <v>7</v>
-      </c>
-      <c r="J2" s="22">
-        <v>3</v>
-      </c>
-      <c r="K2" s="22">
-        <v>3</v>
-      </c>
-      <c r="L2" s="22">
-        <v>0</v>
-      </c>
-      <c r="M2" s="22">
-        <v>0</v>
-      </c>
-      <c r="N2" s="22">
-        <v>0</v>
-      </c>
-      <c r="O2" s="22">
-        <v>0</v>
-      </c>
-      <c r="P2" s="25">
-        <f>SUM(C2:N2)</f>
-        <v>199</v>
-      </c>
-      <c r="Q2" s="20">
-        <f t="shared" ref="Q2:Q17" si="0">S2-P2</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="19">
-        <f>Q2/IBNR!R4</f>
-        <v>0</v>
-      </c>
-      <c r="S2" s="30">
-        <f t="shared" ref="S2:S17" si="1">SUM(C2:O2)</f>
-        <v>199</v>
-      </c>
-      <c r="T2" s="19">
-        <f>S2/IBNR!S4</f>
-        <v>0.9995385395455223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="22">
-        <v>3</v>
-      </c>
-      <c r="D3" s="22">
-        <v>46</v>
-      </c>
-      <c r="E3" s="22">
-        <v>61</v>
-      </c>
-      <c r="F3" s="22">
-        <v>43</v>
-      </c>
-      <c r="G3" s="22">
-        <v>28</v>
-      </c>
-      <c r="H3" s="22">
-        <v>17</v>
-      </c>
-      <c r="I3" s="22">
-        <v>5</v>
-      </c>
-      <c r="J3" s="22">
-        <v>3</v>
-      </c>
-      <c r="K3" s="22">
-        <v>1</v>
-      </c>
-      <c r="L3" s="22">
-        <v>2</v>
-      </c>
-      <c r="M3" s="22">
-        <v>1</v>
-      </c>
-      <c r="N3" s="22">
-        <v>0</v>
-      </c>
-      <c r="O3" s="22">
-        <v>0</v>
-      </c>
-      <c r="P3" s="25">
-        <f>SUM(C3:N3)</f>
-        <v>210</v>
-      </c>
-      <c r="Q3" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="19">
-        <f>Q3/IBNR!R5</f>
-        <v>0</v>
-      </c>
-      <c r="S3" s="30">
-        <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
-      <c r="T3" s="19">
-        <f>S3/IBNR!S5</f>
-        <v>0.99957979461678315</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="22">
-        <v>4</v>
-      </c>
-      <c r="D4" s="22">
-        <v>33</v>
-      </c>
-      <c r="E4" s="22">
-        <v>49</v>
-      </c>
-      <c r="F4" s="22">
-        <v>46</v>
-      </c>
-      <c r="G4" s="22">
-        <v>27</v>
-      </c>
-      <c r="H4" s="22">
-        <v>11</v>
-      </c>
-      <c r="I4" s="22">
-        <v>7</v>
-      </c>
-      <c r="J4" s="22">
-        <v>3</v>
-      </c>
-      <c r="K4" s="22">
-        <v>2</v>
-      </c>
-      <c r="L4" s="22">
-        <v>0</v>
-      </c>
-      <c r="M4" s="22">
-        <v>0</v>
-      </c>
-      <c r="N4" s="22">
-        <v>0</v>
-      </c>
-      <c r="O4" s="22">
-        <v>0</v>
-      </c>
-      <c r="P4" s="25">
-        <f>SUM(C4:N4)</f>
-        <v>182</v>
-      </c>
-      <c r="Q4" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R4" s="19">
-        <f>Q4/IBNR!R6</f>
-        <v>0</v>
-      </c>
-      <c r="S4" s="30">
-        <f t="shared" si="1"/>
-        <v>182</v>
-      </c>
-      <c r="T4" s="19">
-        <f>S4/IBNR!S6</f>
-        <v>0.9995311442736764</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="22">
-        <v>4</v>
-      </c>
-      <c r="D5" s="22">
-        <v>36</v>
-      </c>
-      <c r="E5" s="22">
-        <v>73</v>
-      </c>
-      <c r="F5" s="22">
-        <v>47</v>
-      </c>
-      <c r="G5" s="22">
-        <v>31</v>
-      </c>
-      <c r="H5" s="22">
-        <v>18</v>
-      </c>
-      <c r="I5" s="22">
-        <v>14</v>
-      </c>
-      <c r="J5" s="22">
-        <v>8</v>
-      </c>
-      <c r="K5" s="22">
-        <v>3</v>
-      </c>
-      <c r="L5" s="22">
-        <v>0</v>
-      </c>
-      <c r="M5" s="22">
-        <v>1</v>
-      </c>
-      <c r="N5" s="22">
-        <v>0</v>
-      </c>
-      <c r="O5" s="22">
-        <v>0</v>
-      </c>
-      <c r="P5" s="25">
-        <f>SUM(C5:N5)</f>
-        <v>235</v>
-      </c>
-      <c r="Q5" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="19">
-        <f>Q5/IBNR!R7</f>
-        <v>0</v>
-      </c>
-      <c r="S5" s="30">
-        <f t="shared" si="1"/>
-        <v>235</v>
-      </c>
-      <c r="T5" s="19">
-        <f>S5/IBNR!S7</f>
-        <v>0.99961229542869889</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="22">
-        <v>4</v>
-      </c>
-      <c r="D6" s="22">
-        <v>40</v>
-      </c>
-      <c r="E6" s="22">
-        <v>49</v>
-      </c>
-      <c r="F6" s="22">
-        <v>52</v>
-      </c>
-      <c r="G6" s="22">
-        <v>33</v>
-      </c>
-      <c r="H6" s="22">
-        <v>19</v>
-      </c>
-      <c r="I6" s="22">
-        <v>7</v>
-      </c>
-      <c r="J6" s="22">
-        <v>1</v>
-      </c>
-      <c r="K6" s="22">
-        <v>1</v>
-      </c>
-      <c r="L6" s="22">
-        <v>0</v>
-      </c>
-      <c r="M6" s="22">
-        <v>0</v>
-      </c>
-      <c r="N6" s="22">
-        <v>0</v>
-      </c>
-      <c r="O6" s="22">
-        <v>0</v>
-      </c>
-      <c r="P6" s="25">
-        <f>SUM(C6:N6)</f>
-        <v>206</v>
-      </c>
-      <c r="Q6" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="19">
-        <f>Q6/IBNR!R8</f>
-        <v>0</v>
-      </c>
-      <c r="S6" s="30">
-        <f t="shared" si="1"/>
-        <v>206</v>
-      </c>
-      <c r="T6" s="19">
-        <f>S6/IBNR!S8</f>
-        <v>0.99957806978932506</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="22">
-        <v>2</v>
-      </c>
-      <c r="D7" s="22">
-        <v>30</v>
-      </c>
-      <c r="E7" s="22">
-        <v>58</v>
-      </c>
-      <c r="F7" s="22">
-        <v>39</v>
-      </c>
-      <c r="G7" s="22">
-        <v>35</v>
-      </c>
-      <c r="H7" s="22">
-        <v>9</v>
-      </c>
-      <c r="I7" s="22">
-        <v>12</v>
-      </c>
-      <c r="J7" s="22">
-        <v>5</v>
-      </c>
-      <c r="K7" s="22">
-        <v>5</v>
-      </c>
-      <c r="L7" s="22">
-        <v>1</v>
-      </c>
-      <c r="M7" s="22">
-        <v>0</v>
-      </c>
-      <c r="N7" s="22">
-        <v>0</v>
-      </c>
-      <c r="O7" s="22">
-        <v>0</v>
-      </c>
-      <c r="P7" s="25">
-        <f>SUM(C7:M7)</f>
-        <v>196</v>
-      </c>
-      <c r="Q7" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="19">
-        <f>Q7/IBNR!R9</f>
-        <v>0</v>
-      </c>
-      <c r="S7" s="30">
-        <f t="shared" si="1"/>
-        <v>196</v>
-      </c>
-      <c r="T7" s="19">
-        <f>S7/IBNR!S9</f>
-        <v>0.99884268016011979</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="22">
-        <v>1</v>
-      </c>
-      <c r="D8" s="22">
-        <v>26</v>
-      </c>
-      <c r="E8" s="22">
-        <v>63</v>
-      </c>
-      <c r="F8" s="22">
-        <v>43</v>
-      </c>
-      <c r="G8" s="22">
-        <v>30</v>
-      </c>
-      <c r="H8" s="22">
-        <v>14</v>
-      </c>
-      <c r="I8" s="22">
-        <v>7</v>
-      </c>
-      <c r="J8" s="22">
-        <v>8</v>
-      </c>
-      <c r="K8" s="22">
-        <v>3</v>
-      </c>
-      <c r="L8" s="22">
-        <v>2</v>
-      </c>
-      <c r="M8" s="22">
-        <v>0</v>
-      </c>
-      <c r="N8" s="22">
-        <v>0</v>
-      </c>
-      <c r="O8" s="22">
-        <v>0</v>
-      </c>
-      <c r="P8" s="25">
-        <f>SUM(C8:L8)</f>
-        <v>197</v>
-      </c>
-      <c r="Q8" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="19">
-        <f>Q8/IBNR!R10</f>
-        <v>0</v>
-      </c>
-      <c r="S8" s="30">
-        <f t="shared" si="1"/>
-        <v>197</v>
-      </c>
-      <c r="T8" s="19">
-        <f>S8/IBNR!S10</f>
-        <v>0.9972473094054648</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="22">
-        <v>3</v>
-      </c>
-      <c r="D9" s="22">
-        <v>34</v>
-      </c>
-      <c r="E9" s="22">
-        <v>43</v>
-      </c>
-      <c r="F9" s="22">
-        <v>44</v>
-      </c>
-      <c r="G9" s="22">
-        <v>26</v>
-      </c>
-      <c r="H9" s="22">
-        <v>27</v>
-      </c>
-      <c r="I9" s="22">
-        <v>6</v>
-      </c>
-      <c r="J9" s="22">
-        <v>5</v>
-      </c>
-      <c r="K9" s="22">
-        <v>1</v>
-      </c>
-      <c r="L9" s="22">
-        <v>2</v>
-      </c>
-      <c r="M9" s="22">
-        <v>2</v>
-      </c>
-      <c r="N9" s="22">
-        <v>0</v>
-      </c>
-      <c r="O9" s="22">
-        <v>1</v>
-      </c>
-      <c r="P9" s="25">
-        <f>SUM(C9:K9)</f>
-        <v>189</v>
-      </c>
-      <c r="Q9" s="20">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="R9" s="19">
-        <f>Q9/IBNR!R11</f>
-        <v>3.9309906842211872</v>
-      </c>
-      <c r="S9" s="30">
-        <f t="shared" si="1"/>
-        <v>194</v>
-      </c>
-      <c r="T9" s="19">
-        <f>S9/IBNR!S11</f>
-        <v>1.0195933038023302</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C10" s="22">
-        <v>1</v>
-      </c>
-      <c r="D10" s="22">
-        <v>39</v>
-      </c>
-      <c r="E10" s="22">
-        <v>49</v>
-      </c>
-      <c r="F10" s="22">
-        <v>44</v>
-      </c>
-      <c r="G10" s="22">
-        <v>21</v>
-      </c>
-      <c r="H10" s="22">
-        <v>16</v>
-      </c>
-      <c r="I10" s="22">
-        <v>2</v>
-      </c>
-      <c r="J10" s="22">
-        <v>5</v>
-      </c>
-      <c r="K10" s="22">
-        <v>2</v>
-      </c>
-      <c r="L10" s="22">
-        <v>0</v>
-      </c>
-      <c r="M10" s="22">
-        <v>0</v>
-      </c>
-      <c r="N10" s="22">
-        <v>0</v>
-      </c>
-      <c r="O10" s="22">
-        <v>0</v>
-      </c>
-      <c r="P10" s="25">
-        <f>SUM(C10:J10)</f>
-        <v>177</v>
-      </c>
-      <c r="Q10" s="20">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R10" s="19">
-        <f>Q10/IBNR!R12</f>
-        <v>0.58174990196642862</v>
-      </c>
-      <c r="S10" s="30">
-        <f t="shared" si="1"/>
-        <v>179</v>
-      </c>
-      <c r="T10" s="19">
-        <f>S10/IBNR!S12</f>
-        <v>0.99203103432804052</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C11" s="22">
-        <v>2</v>
-      </c>
-      <c r="D11" s="22">
-        <v>44</v>
-      </c>
-      <c r="E11" s="22">
-        <v>51</v>
-      </c>
-      <c r="F11" s="22">
-        <v>46</v>
-      </c>
-      <c r="G11" s="22">
-        <v>23</v>
-      </c>
-      <c r="H11" s="22">
-        <v>12</v>
-      </c>
-      <c r="I11" s="22">
-        <v>10</v>
-      </c>
-      <c r="J11" s="22">
-        <v>5</v>
-      </c>
-      <c r="K11" s="22">
-        <v>1</v>
-      </c>
-      <c r="L11" s="22">
-        <v>1</v>
-      </c>
-      <c r="M11" s="22">
-        <v>1</v>
-      </c>
-      <c r="N11" s="22">
-        <v>0</v>
-      </c>
-      <c r="O11" s="22">
-        <v>0</v>
-      </c>
-      <c r="P11" s="25">
-        <f>SUM(C11:I11)</f>
-        <v>188</v>
-      </c>
-      <c r="Q11" s="20">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R11" s="19">
-        <f>Q11/IBNR!R13</f>
-        <v>1.132143839047884</v>
-      </c>
-      <c r="S11" s="30">
-        <f t="shared" si="1"/>
-        <v>196</v>
-      </c>
-      <c r="T11" s="19">
-        <f>S11/IBNR!S13</f>
-        <v>1.0047868871215009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="22">
-        <v>3</v>
-      </c>
-      <c r="D12" s="22">
-        <v>42</v>
-      </c>
-      <c r="E12" s="22">
-        <v>58</v>
-      </c>
-      <c r="F12" s="22">
-        <v>38</v>
-      </c>
-      <c r="G12" s="22">
-        <v>26</v>
-      </c>
-      <c r="H12" s="22">
-        <v>15</v>
-      </c>
-      <c r="I12" s="22">
-        <v>10</v>
-      </c>
-      <c r="J12" s="22">
-        <v>6</v>
-      </c>
-      <c r="K12" s="22">
-        <v>1</v>
-      </c>
-      <c r="L12" s="22">
-        <v>2</v>
-      </c>
-      <c r="M12" s="22">
-        <v>1</v>
-      </c>
-      <c r="N12" s="22">
-        <v>0</v>
-      </c>
-      <c r="O12" s="22">
-        <v>0</v>
-      </c>
-      <c r="P12" s="25">
-        <f>SUM(C12:H12)</f>
-        <v>182</v>
-      </c>
-      <c r="Q12" s="20">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="R12" s="19">
-        <f>Q12/IBNR!R14</f>
-        <v>1.275750982600006</v>
-      </c>
-      <c r="S12" s="30">
-        <f t="shared" si="1"/>
-        <v>202</v>
-      </c>
-      <c r="T12" s="19">
-        <f>S12/IBNR!S14</f>
-        <v>1.0218687984532593</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="22">
-        <v>6</v>
-      </c>
-      <c r="D13" s="22">
-        <v>22</v>
-      </c>
-      <c r="E13" s="22">
-        <v>61</v>
-      </c>
-      <c r="F13" s="22">
-        <v>38</v>
-      </c>
-      <c r="G13" s="22">
-        <v>34</v>
-      </c>
-      <c r="H13" s="22">
-        <v>15</v>
-      </c>
-      <c r="I13" s="22">
-        <v>8</v>
-      </c>
-      <c r="J13" s="22">
-        <v>4</v>
-      </c>
-      <c r="K13" s="22">
-        <v>2</v>
-      </c>
-      <c r="L13" s="22">
-        <v>2</v>
-      </c>
-      <c r="M13" s="22">
-        <v>1</v>
-      </c>
-      <c r="N13" s="22">
-        <v>0</v>
-      </c>
-      <c r="O13" s="22">
-        <v>0</v>
-      </c>
-      <c r="P13" s="25">
-        <f>SUM(C13:G13)</f>
-        <v>161</v>
-      </c>
-      <c r="Q13" s="20">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="R13" s="19">
-        <f>Q13/IBNR!R15</f>
-        <v>1.0325805133502648</v>
-      </c>
-      <c r="S13" s="30">
-        <f t="shared" si="1"/>
-        <v>193</v>
-      </c>
-      <c r="T13" s="19">
-        <f>S13/IBNR!S15</f>
-        <v>1.0052590178522891</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="22">
-        <v>4</v>
-      </c>
-      <c r="D14" s="22">
-        <v>33</v>
-      </c>
-      <c r="E14" s="22">
-        <v>57</v>
-      </c>
-      <c r="F14" s="22">
-        <v>45</v>
-      </c>
-      <c r="G14" s="22">
-        <v>26</v>
-      </c>
-      <c r="H14" s="22">
-        <v>21</v>
-      </c>
-      <c r="I14" s="22">
-        <v>16</v>
-      </c>
-      <c r="J14" s="22">
-        <v>3</v>
-      </c>
-      <c r="K14" s="22">
-        <v>1</v>
-      </c>
-      <c r="L14" s="22">
-        <v>2</v>
-      </c>
-      <c r="M14" s="22">
-        <v>1</v>
-      </c>
-      <c r="N14" s="22">
-        <v>1</v>
-      </c>
-      <c r="O14" s="22">
-        <v>0</v>
-      </c>
-      <c r="P14" s="25">
-        <f>SUM(C14:F14)</f>
-        <v>139</v>
-      </c>
-      <c r="Q14" s="20">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="R14" s="19">
-        <f>Q14/IBNR!R16</f>
-        <v>1.1958721446788509</v>
-      </c>
-      <c r="S14" s="30">
-        <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
-      <c r="T14" s="19">
-        <f>S14/IBNR!S16</f>
-        <v>1.0586230383671098</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="22">
-        <v>0</v>
-      </c>
-      <c r="D15" s="22">
-        <v>35</v>
-      </c>
-      <c r="E15" s="22">
-        <v>47</v>
-      </c>
-      <c r="F15" s="22">
-        <v>50</v>
-      </c>
-      <c r="G15" s="22">
-        <v>34</v>
-      </c>
-      <c r="H15" s="22">
-        <v>20</v>
-      </c>
-      <c r="I15" s="22">
-        <v>4</v>
-      </c>
-      <c r="J15" s="22">
-        <v>1</v>
-      </c>
-      <c r="K15" s="22">
-        <v>0</v>
-      </c>
-      <c r="L15" s="22">
-        <v>0</v>
-      </c>
-      <c r="M15" s="22">
-        <v>0</v>
-      </c>
-      <c r="N15" s="22">
-        <v>0</v>
-      </c>
-      <c r="O15" s="22">
-        <v>0</v>
-      </c>
-      <c r="P15" s="25">
-        <f>SUM(C15:E15)</f>
-        <v>82</v>
-      </c>
-      <c r="Q15" s="20">
-        <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-      <c r="R15" s="19">
-        <f>Q15/IBNR!R17</f>
-        <v>1.0687040378896422</v>
-      </c>
-      <c r="S15" s="30">
-        <f t="shared" si="1"/>
-        <v>191</v>
-      </c>
-      <c r="T15" s="19">
-        <f>S15/IBNR!S17</f>
-        <v>1.0380847176515093</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C16" s="22">
-        <v>1</v>
-      </c>
-      <c r="D16" s="22">
-        <v>32</v>
-      </c>
-      <c r="E16" s="22">
-        <v>41</v>
-      </c>
-      <c r="F16" s="22">
-        <v>33</v>
-      </c>
-      <c r="G16" s="22">
-        <v>16</v>
-      </c>
-      <c r="H16" s="22">
-        <v>15</v>
-      </c>
-      <c r="I16" s="22">
-        <v>13</v>
-      </c>
-      <c r="J16" s="22">
-        <v>1</v>
-      </c>
-      <c r="K16" s="22">
-        <v>5</v>
-      </c>
-      <c r="L16" s="22">
-        <v>1</v>
-      </c>
-      <c r="M16" s="22">
-        <v>1</v>
-      </c>
-      <c r="N16" s="22">
-        <v>0</v>
-      </c>
-      <c r="O16" s="22">
-        <v>0</v>
-      </c>
-      <c r="P16" s="25">
-        <f>SUM(C16:D16)</f>
-        <v>33</v>
-      </c>
-      <c r="Q16" s="20">
-        <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="R16" s="19">
-        <f>Q16/IBNR!R18</f>
-        <v>0.90163603931035075</v>
-      </c>
-      <c r="S16" s="30">
-        <f t="shared" si="1"/>
-        <v>159</v>
-      </c>
-      <c r="T16" s="19">
-        <f>S16/IBNR!S18</f>
-        <v>0.92042669916310571</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="22">
-        <v>5</v>
-      </c>
-      <c r="D17" s="22">
-        <v>31</v>
-      </c>
-      <c r="E17" s="22">
-        <v>49</v>
-      </c>
-      <c r="F17" s="22">
-        <v>37</v>
-      </c>
-      <c r="G17" s="22">
-        <v>24</v>
-      </c>
-      <c r="H17" s="22">
-        <v>19</v>
-      </c>
-      <c r="I17" s="22">
-        <v>9</v>
-      </c>
-      <c r="J17" s="22">
-        <v>3</v>
-      </c>
-      <c r="K17" s="22">
-        <v>5</v>
-      </c>
-      <c r="L17" s="22">
-        <v>2</v>
-      </c>
-      <c r="M17" s="22">
-        <v>2</v>
-      </c>
-      <c r="N17" s="22">
-        <v>0</v>
-      </c>
-      <c r="O17" s="22">
-        <v>0</v>
-      </c>
-      <c r="P17" s="25">
-        <f>SUM(C17)</f>
-        <v>5</v>
-      </c>
-      <c r="Q17" s="20">
-        <f t="shared" si="0"/>
-        <v>181</v>
-      </c>
-      <c r="R17" s="19">
-        <f>Q17/IBNR!R19</f>
-        <v>1.0150563777838777</v>
-      </c>
-      <c r="S17" s="30">
-        <f t="shared" si="1"/>
-        <v>186</v>
-      </c>
-      <c r="T17" s="19">
-        <f>S17/IBNR!S19</f>
-        <v>1.0146457087218534</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="P18" s="1"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="3"/>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="20">
-        <f>SUM(Q2:Q17)</f>
-        <v>554</v>
-      </c>
-      <c r="R19" s="19">
-        <f>Q19/IBNR!R21</f>
-        <v>1.0276716005136581</v>
-      </c>
-      <c r="S19" s="3"/>
-      <c r="T19" s="18">
-        <f>AVERAGE(T2:T17)</f>
-        <v>1.0043280649175366</v>
-      </c>
-      <c r="U19" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="O20">
-        <f>IF(IBNR!O4&gt;0,comparison!O2/IBNR!O4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="O21">
-        <f>IF(IBNR!O5&gt;0,comparison!O3/IBNR!O5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="O22">
-        <f>IF(IBNR!O6&gt;0,comparison!O4/IBNR!O6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="O23">
-        <f>IF(IBNR!O7&gt;0,comparison!O5/IBNR!O7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="O24">
-        <f>IF(IBNR!O8&gt;0,comparison!O6/IBNR!O8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="M25" t="str">
-        <f>IF(IBNR!M9&gt;0,comparison!M7/IBNR!M9,"")</f>
-        <v/>
-      </c>
-      <c r="N25">
-        <f>IF(IBNR!N9&gt;0,comparison!N7/IBNR!N9)</f>
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <f>IF(IBNR!O9&gt;0,comparison!O7/IBNR!O9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L26">
-        <f>IF(IBNR!L10&gt;0,comparison!L8/IBNR!L10)</f>
-        <v>1</v>
-      </c>
-      <c r="M26">
-        <f>IF(IBNR!M10&gt;0,comparison!M8/IBNR!M10)</f>
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <f>IF(IBNR!N10&gt;0,comparison!N8/IBNR!N10)</f>
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <f>IF(IBNR!O10&gt;0,comparison!O8/IBNR!O10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K27">
-        <f>IF(IBNR!K11&gt;0,comparison!K9/IBNR!K11)</f>
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <f>IF(IBNR!L11&gt;0,comparison!L9/IBNR!L11)</f>
-        <v>2.6373630727492259</v>
-      </c>
-      <c r="M27">
-        <f>IF(IBNR!M11&gt;0,comparison!M9/IBNR!M11)</f>
-        <v>6.5313622768669006</v>
-      </c>
-      <c r="N27">
-        <f>IF(IBNR!N11&gt;0,comparison!N9/IBNR!N11)</f>
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <f>IF(IBNR!O11&gt;0,comparison!O9/IBNR!O11)</f>
-        <v>11.940803943538015</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J28">
-        <f>IF(IBNR!J12&gt;0,comparison!J10/IBNR!J12)</f>
-        <v>1</v>
-      </c>
-      <c r="K28">
-        <f>IF(IBNR!K12&gt;0,comparison!K10/IBNR!K12)</f>
-        <v>0.97576274803977403</v>
-      </c>
-      <c r="L28">
-        <f>IF(IBNR!L12&gt;0,comparison!L10/IBNR!L12)</f>
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <f>IF(IBNR!M12&gt;0,comparison!M10/IBNR!M12)</f>
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <f>IF(IBNR!N12&gt;0,comparison!N10/IBNR!N12)</f>
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <f>IF(IBNR!O12&gt;0,comparison!O10/IBNR!O12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I29">
-        <f>IF(IBNR!I13&gt;0,comparison!I11/IBNR!I13)</f>
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <f>IF(IBNR!J13&gt;0,comparison!J11/IBNR!J13)</f>
-        <v>1.2263383128987373</v>
-      </c>
-      <c r="K29">
-        <f>IF(IBNR!K13&gt;0,comparison!K11/IBNR!K13)</f>
-        <v>0.56114235537163537</v>
-      </c>
-      <c r="L29">
-        <f>IF(IBNR!L13&gt;0,comparison!L11/IBNR!L13)</f>
-        <v>1.3896547084076922</v>
-      </c>
-      <c r="M29">
-        <f>IF(IBNR!M13&gt;0,comparison!M11/IBNR!M13)</f>
-        <v>3.4414443859271779</v>
-      </c>
-      <c r="N29">
-        <f>IF(IBNR!N13&gt;0,comparison!N11/IBNR!N13)</f>
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <f>IF(IBNR!O13&gt;0,comparison!O11/IBNR!O13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H30">
-        <f>IF(IBNR!H14&gt;0,comparison!H12/IBNR!H14)</f>
-        <v>1</v>
-      </c>
-      <c r="I30">
-        <f>IF(IBNR!I14&gt;0,comparison!I12/IBNR!I14)</f>
-        <v>1.2850636839076144</v>
-      </c>
-      <c r="J30">
-        <f>IF(IBNR!J14&gt;0,comparison!J12/IBNR!J14)</f>
-        <v>1.3170731707317076</v>
-      </c>
-      <c r="K30">
-        <f>IF(IBNR!K14&gt;0,comparison!K12/IBNR!K14)</f>
-        <v>0.50221700206189723</v>
-      </c>
-      <c r="L30">
-        <f>IF(IBNR!L14&gt;0,comparison!L12/IBNR!L14)</f>
-        <v>2.4874551524291828</v>
-      </c>
-      <c r="M30">
-        <f>IF(IBNR!M14&gt;0,comparison!M12/IBNR!M14)</f>
-        <v>3.0800595708346319</v>
-      </c>
-      <c r="N30">
-        <f>IF(IBNR!N14&gt;0,comparison!N12/IBNR!N14)</f>
-        <v>0</v>
-      </c>
-      <c r="O30">
-        <f>IF(IBNR!O14&gt;0,comparison!O12/IBNR!O14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G31">
-        <f>IF(IBNR!G15&gt;0,comparison!G13/IBNR!G15)</f>
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <f>IF(IBNR!H15&gt;0,comparison!H13/IBNR!H15)</f>
-        <v>0.95643103812812735</v>
-      </c>
-      <c r="I31">
-        <f>IF(IBNR!I15&gt;0,comparison!I13/IBNR!I15)</f>
-        <v>1.0529026967112807</v>
-      </c>
-      <c r="J31">
-        <f>IF(IBNR!J15&gt;0,comparison!J13/IBNR!J15)</f>
-        <v>0.89927442935011492</v>
-      </c>
-      <c r="K31">
-        <f>IF(IBNR!K15&gt;0,comparison!K13/IBNR!K15)</f>
-        <v>1.02871484586137</v>
-      </c>
-      <c r="L31">
-        <f>IF(IBNR!L15&gt;0,comparison!L13/IBNR!L15)</f>
-        <v>2.5475860367256953</v>
-      </c>
-      <c r="M31">
-        <f>IF(IBNR!M15&gt;0,comparison!M13/IBNR!M15)</f>
-        <v>3.1545158702776006</v>
-      </c>
-      <c r="N31">
-        <f>IF(IBNR!N15&gt;0,comparison!N13/IBNR!N15)</f>
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <f>IF(IBNR!O15&gt;0,comparison!O13/IBNR!O15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F32">
-        <f>IF(IBNR!F16&gt;0,comparison!F14/IBNR!F16)</f>
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <f>IF(IBNR!G16&gt;0,comparison!G14/IBNR!G16)</f>
-        <v>0.91072281348069339</v>
-      </c>
-      <c r="H32">
-        <f>IF(IBNR!H16&gt;0,comparison!H14/IBNR!H16)</f>
-        <v>1.3463095238095237</v>
-      </c>
-      <c r="I32">
-        <f>IF(IBNR!I16&gt;0,comparison!I14/IBNR!I16)</f>
-        <v>2.1172954030096887</v>
-      </c>
-      <c r="J32">
-        <f>IF(IBNR!J16&gt;0,comparison!J14/IBNR!J16)</f>
-        <v>0.67813588850174222</v>
-      </c>
-      <c r="K32">
-        <f>IF(IBNR!K16&gt;0,comparison!K14/IBNR!K16)</f>
-        <v>0.51716393664707272</v>
-      </c>
-      <c r="L32">
-        <f>IF(IBNR!L16&gt;0,comparison!L14/IBNR!L16)</f>
-        <v>2.5614865557752897</v>
-      </c>
-      <c r="M32">
-        <f>IF(IBNR!M16&gt;0,comparison!M14/IBNR!M16)</f>
-        <v>3.1717280104428056</v>
-      </c>
-      <c r="N32">
-        <f>IF(IBNR!N16&gt;0,comparison!N14/IBNR!N16)</f>
-        <v>7.8547033944377995</v>
-      </c>
-      <c r="O32">
-        <f>IF(IBNR!O16&gt;0,comparison!O14/IBNR!O16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="E33">
-        <f>IF(IBNR!E17&gt;0,comparison!E15/IBNR!E17)</f>
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <f>IF(IBNR!F17&gt;0,comparison!F15/IBNR!F17)</f>
-        <v>1.1714898366303133</v>
-      </c>
-      <c r="G33">
-        <f>IF(IBNR!G17&gt;0,comparison!G15/IBNR!G17)</f>
-        <v>1.1921278841803653</v>
-      </c>
-      <c r="H33">
-        <f>IF(IBNR!H17&gt;0,comparison!H15/IBNR!H17)</f>
-        <v>1.2834728330259613</v>
-      </c>
-      <c r="I33">
-        <f>IF(IBNR!I17&gt;0,comparison!I15/IBNR!I17)</f>
-        <v>0.529849495092792</v>
-      </c>
-      <c r="J33">
-        <f>IF(IBNR!J17&gt;0,comparison!J15/IBNR!J17)</f>
-        <v>0.2262697701455664</v>
-      </c>
-      <c r="K33">
-        <f>IF(IBNR!K17&gt;0,comparison!K15/IBNR!K17)</f>
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <f>IF(IBNR!L17&gt;0,comparison!L15/IBNR!L17)</f>
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <f>IF(IBNR!M17&gt;0,comparison!M15/IBNR!M17)</f>
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <f>IF(IBNR!N17&gt;0,comparison!N15/IBNR!N17)</f>
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <f>IF(IBNR!O17&gt;0,comparison!O15/IBNR!O17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D34">
-        <f>IF(IBNR!D18&gt;0,comparison!D16/IBNR!D18)</f>
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <f>IF(IBNR!E18&gt;0,comparison!E16/IBNR!E18)</f>
-        <v>0.85177360612113462</v>
-      </c>
-      <c r="F34">
-        <f>IF(IBNR!F18&gt;0,comparison!F16/IBNR!F18)</f>
-        <v>0.86080218377140827</v>
-      </c>
-      <c r="G34">
-        <f>IF(IBNR!G18&gt;0,comparison!G16/IBNR!G18)</f>
-        <v>0.62457530874757083</v>
-      </c>
-      <c r="H34">
-        <f>IF(IBNR!H18&gt;0,comparison!H16/IBNR!H18)</f>
-        <v>1.0716891731817104</v>
-      </c>
-      <c r="I34">
-        <f>IF(IBNR!I18&gt;0,comparison!I16/IBNR!I18)</f>
-        <v>1.9171530514814095</v>
-      </c>
-      <c r="J34">
-        <f>IF(IBNR!J18&gt;0,comparison!J16/IBNR!J18)</f>
-        <v>0.25191117582817624</v>
-      </c>
-      <c r="K34">
-        <f>IF(IBNR!K18&gt;0,comparison!K16/IBNR!K18)</f>
-        <v>2.8817094977349327</v>
-      </c>
-      <c r="L34">
-        <f>IF(IBNR!L18&gt;0,comparison!L16/IBNR!L18)</f>
-        <v>1.4272959912777732</v>
-      </c>
-      <c r="M34">
-        <f>IF(IBNR!M18&gt;0,comparison!M16/IBNR!M18)</f>
-        <v>3.534662061388997</v>
-      </c>
-      <c r="N34">
-        <f>IF(IBNR!N18&gt;0,comparison!N16/IBNR!N18)</f>
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <f>IF(IBNR!O18&gt;0,comparison!O16/IBNR!O18)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <f>IF(IBNR!C19&gt;0,comparison!C17/IBNR!C19)</f>
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <f>IF(IBNR!D19&gt;0,comparison!D17/IBNR!D19)</f>
-        <v>0.93481267224716125</v>
-      </c>
-      <c r="E35">
-        <f>IF(IBNR!E19&gt;0,comparison!E17/IBNR!E19)</f>
-        <v>0.98004989966359224</v>
-      </c>
-      <c r="F35">
-        <f>IF(IBNR!F19&gt;0,comparison!F17/IBNR!F19)</f>
-        <v>0.92918658484318972</v>
-      </c>
-      <c r="G35">
-        <f>IF(IBNR!G19&gt;0,comparison!G17/IBNR!G19)</f>
-        <v>0.9019612029199221</v>
-      </c>
-      <c r="H35">
-        <f>IF(IBNR!H19&gt;0,comparison!H17/IBNR!H19)</f>
-        <v>1.3069018474872651</v>
-      </c>
-      <c r="I35">
-        <f>IF(IBNR!I19&gt;0,comparison!I17/IBNR!I19)</f>
-        <v>1.2778142559941388</v>
-      </c>
-      <c r="J35">
-        <f>IF(IBNR!J19&gt;0,comparison!J17/IBNR!J19)</f>
-        <v>0.72757953763678151</v>
-      </c>
-      <c r="K35">
-        <f>IF(IBNR!K19&gt;0,comparison!K17/IBNR!K19)</f>
-        <v>2.7743547000545465</v>
-      </c>
-      <c r="L35">
-        <f>IF(IBNR!L19&gt;0,comparison!L17/IBNR!L19)</f>
-        <v>2.7482474169467714</v>
-      </c>
-      <c r="M35">
-        <f>IF(IBNR!M19&gt;0,comparison!M17/IBNR!M19)</f>
-        <v>6.8059645226745031</v>
-      </c>
-      <c r="N35">
-        <f>IF(IBNR!N19&gt;0,comparison!N17/IBNR!N19)</f>
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <f>IF(IBNR!O19&gt;0,comparison!O17/IBNR!O19)</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C20:O35">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>